<commit_message>
hard_first and easy_first: uniformização
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,32 +436,62 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>a11</t>
+          <t>g</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>a12</t>
+          <t>n</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>a21</t>
+          <t>sqgrupos</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>a22</t>
+          <t>sqerros</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>dfgrupos</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>solucaounica</t>
+          <t>dferros</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>sqtotal</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>dftotal</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>msqgrupos</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>msqerros</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>sig</t>
         </is>
       </c>
     </row>
@@ -482,12 +512,28 @@
         <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>tem zero ou infinitas soluções</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12</v>
+      </c>
+      <c r="H2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" t="n">
+        <v>15</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.333</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4.003</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.035</v>
       </c>
     </row>
     <row r="3">
@@ -501,18 +547,34 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>1000</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>-20</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>tem solução única</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="I3" t="n">
+        <v>23</v>
+      </c>
+      <c r="J3" t="n">
+        <v>333.333</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>66.667</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -520,24 +582,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E4" t="n">
+        <v>480</v>
+      </c>
+      <c r="F4" t="n">
         <v>3</v>
       </c>
-      <c r="E4" t="n">
-        <v>4</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>tem solução única</t>
-        </is>
+      <c r="G4" t="n">
+        <v>16</v>
+      </c>
+      <c r="H4" t="n">
+        <v>980</v>
+      </c>
+      <c r="I4" t="n">
+        <v>19</v>
+      </c>
+      <c r="J4" t="n">
+        <v>166.667</v>
+      </c>
+      <c r="K4" t="n">
+        <v>30</v>
+      </c>
+      <c r="L4" t="n">
+        <v>5.556</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.008</v>
       </c>
     </row>
     <row r="5">
@@ -545,24 +623,81 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>180</v>
+      </c>
+      <c r="E5" t="n">
+        <v>170</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" t="n">
+        <v>350</v>
+      </c>
+      <c r="I5" t="n">
+        <v>24</v>
+      </c>
+      <c r="J5" t="n">
+        <v>45</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>5.294</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>200</v>
+      </c>
+      <c r="E6" t="n">
+        <v>120</v>
+      </c>
+      <c r="F6" t="n">
         <v>3</v>
       </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>tem zero ou infinitas soluções</t>
-        </is>
+      <c r="G6" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" t="n">
+        <v>320</v>
+      </c>
+      <c r="I6" t="n">
+        <v>15</v>
+      </c>
+      <c r="J6" t="n">
+        <v>66.667</v>
+      </c>
+      <c r="K6" t="n">
+        <v>10</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6.667</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>